<commit_message>
exercicios org de projetos
</commit_message>
<xml_diff>
--- a/tab_exercicios.xlsx
+++ b/tab_exercicios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/william/Documents/curso-r/202104-r4ds-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F68963-EDA4-9642-B524-5125FF6D8787}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F797A2EC-9E38-0B4E-92D5-E2A086E23374}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44500" yWindow="60" windowWidth="30020" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1120" yWindow="1060" windowWidth="27160" windowHeight="15960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>aula</t>
   </si>
@@ -48,17 +48,32 @@
     <t>https://livro.curso-r.com/7-2-dplyr.html#exerc%C3%ADcios-17</t>
   </si>
   <si>
-    <t>não</t>
-  </si>
-  <si>
     <t>https://livro.curso-r.com/7-3-tidyr.html#exerc%C3%ADcios-18</t>
+  </si>
+  <si>
+    <t>Faça um mini relatório com um gráfico mostrando a frequência das espécies dos personagens do Star Wars. Use a base "starwars" do pacote dplyr. Faça isso seguindo o modelo de organização de projetos visto na primeira aula.</t>
+  </si>
+  <si>
+    <t>https://dplyr.tidyverse.org/reference/starwars.html</t>
+  </si>
+  <si>
+    <t>nao</t>
+  </si>
+  <si>
+    <t>Reorganize alguma análise que você já fez no R seguindo o modelo de organização de projetos visto na primeira aula.</t>
+  </si>
+  <si>
+    <t>sim</t>
+  </si>
+  <si>
+    <t>https://curso-r.github.io/main-r4ds-2/slides/02-organizacao-projeto.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -70,6 +85,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -92,16 +115,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -414,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -441,35 +467,66 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
+      <c r="D5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{6237448C-3190-FA45-A26E-C716B76A2DC5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>